<commit_message>
Updating classification and label names
</commit_message>
<xml_diff>
--- a/DATA/spClassification.xlsx
+++ b/DATA/spClassification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahipp\Documents\CODE\2021-oak-classification\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5008CB-68F6-4A31-A172-335D7413E091}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50742C8E-3B7F-4571-9836-0808B5F9C874}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18270" windowHeight="8565" xr2:uid="{EFBBD03D-450F-48B5-9E09-34D03F002882}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$183</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$E$183</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -613,9 +613,6 @@
     <t>clade</t>
   </si>
   <si>
-    <t>Velutinae</t>
-  </si>
-  <si>
     <t>Phellos</t>
   </si>
   <si>
@@ -626,6 +623,9 @@
   </si>
   <si>
     <t>REMAINDERS</t>
+  </si>
+  <si>
+    <t>Coccineae</t>
   </si>
 </sst>
 </file>
@@ -988,8 +988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AA191D6-CE6D-47A9-8F77-E166988EFEDF}">
   <dimension ref="A1:E183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,10 +1164,10 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1181,10 +1181,10 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1198,10 +1198,10 @@
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1215,10 +1215,10 @@
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1232,10 +1232,10 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1249,10 +1249,10 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1266,10 +1266,10 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1283,10 +1283,10 @@
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1300,10 +1300,10 @@
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1317,10 +1317,10 @@
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1334,10 +1334,10 @@
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1351,10 +1351,10 @@
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E21" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1368,10 +1368,10 @@
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1385,10 +1385,10 @@
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1402,10 +1402,10 @@
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E24" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1419,10 +1419,10 @@
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1436,10 +1436,10 @@
         <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="E26" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1453,10 +1453,10 @@
         <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="E27" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1470,10 +1470,10 @@
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="E28" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1487,10 +1487,10 @@
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="E29" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1504,10 +1504,10 @@
         <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="E30" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1521,10 +1521,10 @@
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="E31" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1538,10 +1538,10 @@
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="E32" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1555,7 +1555,7 @@
         <v>4</v>
       </c>
       <c r="E33" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1569,7 +1569,7 @@
         <v>4</v>
       </c>
       <c r="E34" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1583,7 +1583,7 @@
         <v>4</v>
       </c>
       <c r="E35" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1597,7 +1597,7 @@
         <v>4</v>
       </c>
       <c r="E36" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1611,7 +1611,7 @@
         <v>4</v>
       </c>
       <c r="E37" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1625,7 +1625,7 @@
         <v>4</v>
       </c>
       <c r="E38" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1639,7 +1639,7 @@
         <v>4</v>
       </c>
       <c r="E39" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1653,7 +1653,7 @@
         <v>4</v>
       </c>
       <c r="E40" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1667,7 +1667,7 @@
         <v>4</v>
       </c>
       <c r="E41" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1681,7 +1681,7 @@
         <v>4</v>
       </c>
       <c r="E42" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1695,7 +1695,7 @@
         <v>4</v>
       </c>
       <c r="E43" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1709,7 +1709,7 @@
         <v>4</v>
       </c>
       <c r="E44" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1723,7 +1723,7 @@
         <v>7</v>
       </c>
       <c r="E45" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1737,7 +1737,7 @@
         <v>4</v>
       </c>
       <c r="E46" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1751,7 +1751,7 @@
         <v>4</v>
       </c>
       <c r="E47" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1765,7 +1765,7 @@
         <v>4</v>
       </c>
       <c r="E48" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1779,7 +1779,7 @@
         <v>4</v>
       </c>
       <c r="E49" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1793,7 +1793,7 @@
         <v>4</v>
       </c>
       <c r="E50" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1807,7 +1807,7 @@
         <v>4</v>
       </c>
       <c r="E51" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1821,7 +1821,7 @@
         <v>4</v>
       </c>
       <c r="E52" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1835,7 +1835,7 @@
         <v>4</v>
       </c>
       <c r="E53" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1849,7 +1849,7 @@
         <v>4</v>
       </c>
       <c r="E54" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1863,7 +1863,7 @@
         <v>4</v>
       </c>
       <c r="E55" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1877,7 +1877,7 @@
         <v>4</v>
       </c>
       <c r="E56" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1891,7 +1891,7 @@
         <v>4</v>
       </c>
       <c r="E57" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1905,7 +1905,7 @@
         <v>4</v>
       </c>
       <c r="E58" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1919,7 +1919,7 @@
         <v>4</v>
       </c>
       <c r="E59" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -1933,7 +1933,7 @@
         <v>4</v>
       </c>
       <c r="E60" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -1947,7 +1947,7 @@
         <v>4</v>
       </c>
       <c r="E61" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1961,7 +1961,7 @@
         <v>4</v>
       </c>
       <c r="E62" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1975,7 +1975,7 @@
         <v>4</v>
       </c>
       <c r="E63" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -1989,7 +1989,7 @@
         <v>4</v>
       </c>
       <c r="E64" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2003,7 +2003,7 @@
         <v>4</v>
       </c>
       <c r="E65" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -2017,7 +2017,7 @@
         <v>4</v>
       </c>
       <c r="E66" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -2031,7 +2031,7 @@
         <v>4</v>
       </c>
       <c r="E67" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -2045,7 +2045,7 @@
         <v>4</v>
       </c>
       <c r="E68" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2059,7 +2059,7 @@
         <v>4</v>
       </c>
       <c r="E69" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -2073,7 +2073,7 @@
         <v>4</v>
       </c>
       <c r="E70" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2087,7 +2087,7 @@
         <v>4</v>
       </c>
       <c r="E71" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2101,7 +2101,7 @@
         <v>4</v>
       </c>
       <c r="E72" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2115,7 +2115,7 @@
         <v>4</v>
       </c>
       <c r="E73" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2129,7 +2129,7 @@
         <v>4</v>
       </c>
       <c r="E74" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2143,7 +2143,7 @@
         <v>4</v>
       </c>
       <c r="E75" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2255,7 +2255,7 @@
         <v>7</v>
       </c>
       <c r="E83" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -2269,7 +2269,7 @@
         <v>7</v>
       </c>
       <c r="E84" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -2283,7 +2283,7 @@
         <v>7</v>
       </c>
       <c r="E85" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -2297,7 +2297,7 @@
         <v>7</v>
       </c>
       <c r="E86" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -2311,7 +2311,7 @@
         <v>7</v>
       </c>
       <c r="E87" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -2325,7 +2325,7 @@
         <v>7</v>
       </c>
       <c r="E88" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -2339,7 +2339,7 @@
         <v>7</v>
       </c>
       <c r="E89" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -2353,7 +2353,7 @@
         <v>7</v>
       </c>
       <c r="E90" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -2367,7 +2367,7 @@
         <v>7</v>
       </c>
       <c r="E91" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -2381,7 +2381,7 @@
         <v>7</v>
       </c>
       <c r="E92" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -2395,7 +2395,7 @@
         <v>7</v>
       </c>
       <c r="E93" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -2409,7 +2409,7 @@
         <v>7</v>
       </c>
       <c r="E94" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -2423,7 +2423,7 @@
         <v>7</v>
       </c>
       <c r="E95" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -2437,7 +2437,7 @@
         <v>7</v>
       </c>
       <c r="E96" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2451,7 +2451,7 @@
         <v>7</v>
       </c>
       <c r="E97" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2465,7 +2465,7 @@
         <v>7</v>
       </c>
       <c r="E98" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2479,7 +2479,7 @@
         <v>7</v>
       </c>
       <c r="E99" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2493,7 +2493,7 @@
         <v>7</v>
       </c>
       <c r="E100" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2507,7 +2507,7 @@
         <v>7</v>
       </c>
       <c r="E101" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2521,7 +2521,7 @@
         <v>7</v>
       </c>
       <c r="E102" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2535,7 +2535,7 @@
         <v>7</v>
       </c>
       <c r="E103" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -2549,7 +2549,7 @@
         <v>7</v>
       </c>
       <c r="E104" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -2563,7 +2563,7 @@
         <v>7</v>
       </c>
       <c r="E105" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -2577,7 +2577,7 @@
         <v>7</v>
       </c>
       <c r="E106" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -2795,10 +2795,10 @@
         <v>7</v>
       </c>
       <c r="D119" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E119" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -2812,10 +2812,10 @@
         <v>7</v>
       </c>
       <c r="D120" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E120" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -2829,10 +2829,10 @@
         <v>7</v>
       </c>
       <c r="D121" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E121" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -2846,10 +2846,10 @@
         <v>7</v>
       </c>
       <c r="D122" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E122" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -2863,10 +2863,10 @@
         <v>7</v>
       </c>
       <c r="D123" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E123" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -3131,10 +3131,10 @@
         <v>7</v>
       </c>
       <c r="D140" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E140" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -3148,10 +3148,10 @@
         <v>7</v>
       </c>
       <c r="D141" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E141" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -3165,10 +3165,10 @@
         <v>7</v>
       </c>
       <c r="D142" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E142" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -3182,10 +3182,10 @@
         <v>7</v>
       </c>
       <c r="D143" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E143" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -3199,10 +3199,10 @@
         <v>7</v>
       </c>
       <c r="D144" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E144" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -3216,10 +3216,10 @@
         <v>7</v>
       </c>
       <c r="D145" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E145" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -3233,7 +3233,7 @@
         <v>7</v>
       </c>
       <c r="E146" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -3247,7 +3247,7 @@
         <v>7</v>
       </c>
       <c r="E147" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -3261,7 +3261,7 @@
         <v>7</v>
       </c>
       <c r="E148" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -3275,7 +3275,7 @@
         <v>7</v>
       </c>
       <c r="E149" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -3289,7 +3289,7 @@
         <v>7</v>
       </c>
       <c r="E150" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -3303,7 +3303,7 @@
         <v>7</v>
       </c>
       <c r="E151" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -3317,7 +3317,7 @@
         <v>7</v>
       </c>
       <c r="E152" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -3331,7 +3331,7 @@
         <v>7</v>
       </c>
       <c r="E153" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -3345,7 +3345,7 @@
         <v>7</v>
       </c>
       <c r="E154" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -3359,7 +3359,7 @@
         <v>7</v>
       </c>
       <c r="E155" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -3373,7 +3373,7 @@
         <v>7</v>
       </c>
       <c r="E156" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -3387,7 +3387,7 @@
         <v>7</v>
       </c>
       <c r="E157" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -3401,7 +3401,7 @@
         <v>7</v>
       </c>
       <c r="E158" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -3415,7 +3415,7 @@
         <v>7</v>
       </c>
       <c r="E159" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -3429,7 +3429,7 @@
         <v>7</v>
       </c>
       <c r="E160" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -3443,7 +3443,7 @@
         <v>7</v>
       </c>
       <c r="E161" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -3457,7 +3457,7 @@
         <v>7</v>
       </c>
       <c r="E162" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -3471,7 +3471,7 @@
         <v>7</v>
       </c>
       <c r="E163" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -3485,7 +3485,7 @@
         <v>7</v>
       </c>
       <c r="E164" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -3499,7 +3499,7 @@
         <v>7</v>
       </c>
       <c r="E165" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -3513,7 +3513,7 @@
         <v>7</v>
       </c>
       <c r="E166" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -3527,7 +3527,7 @@
         <v>7</v>
       </c>
       <c r="E167" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -3541,7 +3541,7 @@
         <v>7</v>
       </c>
       <c r="E168" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -3555,7 +3555,7 @@
         <v>7</v>
       </c>
       <c r="E169" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -3569,7 +3569,7 @@
         <v>7</v>
       </c>
       <c r="E170" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -3583,7 +3583,7 @@
         <v>7</v>
       </c>
       <c r="E171" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -3597,7 +3597,7 @@
         <v>7</v>
       </c>
       <c r="E172" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -3611,7 +3611,7 @@
         <v>7</v>
       </c>
       <c r="E173" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -3625,7 +3625,7 @@
         <v>7</v>
       </c>
       <c r="E174" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
@@ -3639,7 +3639,7 @@
         <v>7</v>
       </c>
       <c r="E175" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
@@ -3653,7 +3653,7 @@
         <v>7</v>
       </c>
       <c r="E176" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -3667,7 +3667,7 @@
         <v>7</v>
       </c>
       <c r="E177" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -3681,7 +3681,7 @@
         <v>7</v>
       </c>
       <c r="E178" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
@@ -3712,7 +3712,7 @@
         <v>7</v>
       </c>
       <c r="E180" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
@@ -3743,10 +3743,10 @@
         <v>4</v>
       </c>
       <c r="D182" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E182" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
@@ -3767,6 +3767,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="E1:E183" xr:uid="{D4F52A60-FC7D-452B-ACC0-84CAF00B5A9F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated data and maps v1 layout working
</commit_message>
<xml_diff>
--- a/DATA/spClassification.xlsx
+++ b/DATA/spClassification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahipp\Documents\CODE\2021-oak-classification\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50742C8E-3B7F-4571-9836-0808B5F9C874}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56753E8-F7AC-4488-892A-03295B580AAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18270" windowHeight="8565" xr2:uid="{EFBBD03D-450F-48B5-9E09-34D03F002882}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="198">
   <si>
     <t>subgenus</t>
   </si>
@@ -620,9 +620,6 @@
   </si>
   <si>
     <t>Polymorphae</t>
-  </si>
-  <si>
-    <t>REMAINDERS</t>
   </si>
   <si>
     <t>Coccineae</t>
@@ -989,7 +986,7 @@
   <dimension ref="A1:E183"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="H182" sqref="H182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,6 +995,7 @@
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1436,10 +1434,10 @@
         <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E26" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1453,10 +1451,10 @@
         <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1470,10 +1468,10 @@
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1487,10 +1485,10 @@
         <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E29" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1504,10 +1502,10 @@
         <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1521,10 +1519,10 @@
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E31" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1538,13 +1536,13 @@
         <v>4</v>
       </c>
       <c r="D32" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E32" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -1554,11 +1552,8 @@
       <c r="C33" t="s">
         <v>4</v>
       </c>
-      <c r="E33" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -1568,11 +1563,8 @@
       <c r="C34" t="s">
         <v>4</v>
       </c>
-      <c r="E34" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>46</v>
       </c>
@@ -1582,11 +1574,8 @@
       <c r="C35" t="s">
         <v>4</v>
       </c>
-      <c r="E35" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>47</v>
       </c>
@@ -1596,11 +1585,8 @@
       <c r="C36" t="s">
         <v>4</v>
       </c>
-      <c r="E36" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -1610,11 +1596,8 @@
       <c r="C37" t="s">
         <v>4</v>
       </c>
-      <c r="E37" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>49</v>
       </c>
@@ -1624,11 +1607,8 @@
       <c r="C38" t="s">
         <v>4</v>
       </c>
-      <c r="E38" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>50</v>
       </c>
@@ -1638,11 +1618,8 @@
       <c r="C39" t="s">
         <v>4</v>
       </c>
-      <c r="E39" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>51</v>
       </c>
@@ -1652,11 +1629,8 @@
       <c r="C40" t="s">
         <v>4</v>
       </c>
-      <c r="E40" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>52</v>
       </c>
@@ -1666,11 +1640,8 @@
       <c r="C41" t="s">
         <v>4</v>
       </c>
-      <c r="E41" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>53</v>
       </c>
@@ -1680,11 +1651,8 @@
       <c r="C42" t="s">
         <v>4</v>
       </c>
-      <c r="E42" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>54</v>
       </c>
@@ -1694,11 +1662,8 @@
       <c r="C43" t="s">
         <v>4</v>
       </c>
-      <c r="E43" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>55</v>
       </c>
@@ -1708,11 +1673,8 @@
       <c r="C44" t="s">
         <v>4</v>
       </c>
-      <c r="E44" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>56</v>
       </c>
@@ -1722,11 +1684,8 @@
       <c r="C45" t="s">
         <v>7</v>
       </c>
-      <c r="E45" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>57</v>
       </c>
@@ -1736,11 +1695,8 @@
       <c r="C46" t="s">
         <v>4</v>
       </c>
-      <c r="E46" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>58</v>
       </c>
@@ -1750,11 +1706,8 @@
       <c r="C47" t="s">
         <v>4</v>
       </c>
-      <c r="E47" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>59</v>
       </c>
@@ -1764,11 +1717,8 @@
       <c r="C48" t="s">
         <v>4</v>
       </c>
-      <c r="E48" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>60</v>
       </c>
@@ -1778,11 +1728,8 @@
       <c r="C49" t="s">
         <v>4</v>
       </c>
-      <c r="E49" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>61</v>
       </c>
@@ -1792,11 +1739,8 @@
       <c r="C50" t="s">
         <v>4</v>
       </c>
-      <c r="E50" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>62</v>
       </c>
@@ -1806,11 +1750,8 @@
       <c r="C51" t="s">
         <v>4</v>
       </c>
-      <c r="E51" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>63</v>
       </c>
@@ -1820,11 +1761,8 @@
       <c r="C52" t="s">
         <v>4</v>
       </c>
-      <c r="E52" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>64</v>
       </c>
@@ -1834,11 +1772,8 @@
       <c r="C53" t="s">
         <v>4</v>
       </c>
-      <c r="E53" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>65</v>
       </c>
@@ -1848,11 +1783,8 @@
       <c r="C54" t="s">
         <v>4</v>
       </c>
-      <c r="E54" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>66</v>
       </c>
@@ -1862,11 +1794,8 @@
       <c r="C55" t="s">
         <v>4</v>
       </c>
-      <c r="E55" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>67</v>
       </c>
@@ -1876,11 +1805,8 @@
       <c r="C56" t="s">
         <v>4</v>
       </c>
-      <c r="E56" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>68</v>
       </c>
@@ -1890,11 +1816,8 @@
       <c r="C57" t="s">
         <v>4</v>
       </c>
-      <c r="E57" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>69</v>
       </c>
@@ -1904,11 +1827,8 @@
       <c r="C58" t="s">
         <v>4</v>
       </c>
-      <c r="E58" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>70</v>
       </c>
@@ -1918,11 +1838,8 @@
       <c r="C59" t="s">
         <v>4</v>
       </c>
-      <c r="E59" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>71</v>
       </c>
@@ -1932,11 +1849,8 @@
       <c r="C60" t="s">
         <v>4</v>
       </c>
-      <c r="E60" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>72</v>
       </c>
@@ -1946,11 +1860,8 @@
       <c r="C61" t="s">
         <v>4</v>
       </c>
-      <c r="E61" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>73</v>
       </c>
@@ -1960,11 +1871,8 @@
       <c r="C62" t="s">
         <v>4</v>
       </c>
-      <c r="E62" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>74</v>
       </c>
@@ -1974,11 +1882,8 @@
       <c r="C63" t="s">
         <v>4</v>
       </c>
-      <c r="E63" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>75</v>
       </c>
@@ -1988,11 +1893,8 @@
       <c r="C64" t="s">
         <v>4</v>
       </c>
-      <c r="E64" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>76</v>
       </c>
@@ -2002,11 +1904,8 @@
       <c r="C65" t="s">
         <v>4</v>
       </c>
-      <c r="E65" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>77</v>
       </c>
@@ -2016,11 +1915,8 @@
       <c r="C66" t="s">
         <v>4</v>
       </c>
-      <c r="E66" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>78</v>
       </c>
@@ -2030,11 +1926,8 @@
       <c r="C67" t="s">
         <v>4</v>
       </c>
-      <c r="E67" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>79</v>
       </c>
@@ -2044,11 +1937,8 @@
       <c r="C68" t="s">
         <v>4</v>
       </c>
-      <c r="E68" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>80</v>
       </c>
@@ -2058,11 +1948,8 @@
       <c r="C69" t="s">
         <v>4</v>
       </c>
-      <c r="E69" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>81</v>
       </c>
@@ -2072,11 +1959,8 @@
       <c r="C70" t="s">
         <v>4</v>
       </c>
-      <c r="E70" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>82</v>
       </c>
@@ -2086,11 +1970,8 @@
       <c r="C71" t="s">
         <v>4</v>
       </c>
-      <c r="E71" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>83</v>
       </c>
@@ -2100,11 +1981,8 @@
       <c r="C72" t="s">
         <v>4</v>
       </c>
-      <c r="E72" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>84</v>
       </c>
@@ -2114,11 +1992,8 @@
       <c r="C73" t="s">
         <v>4</v>
       </c>
-      <c r="E73" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>85</v>
       </c>
@@ -2128,11 +2003,8 @@
       <c r="C74" t="s">
         <v>4</v>
       </c>
-      <c r="E74" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>86</v>
       </c>
@@ -2142,11 +2014,8 @@
       <c r="C75" t="s">
         <v>4</v>
       </c>
-      <c r="E75" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>87</v>
       </c>
@@ -2156,11 +2025,8 @@
       <c r="C76" t="s">
         <v>8</v>
       </c>
-      <c r="E76" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>88</v>
       </c>
@@ -2170,11 +2036,8 @@
       <c r="C77" t="s">
         <v>8</v>
       </c>
-      <c r="E77" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>89</v>
       </c>
@@ -2184,11 +2047,8 @@
       <c r="C78" t="s">
         <v>8</v>
       </c>
-      <c r="E78" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>90</v>
       </c>
@@ -2198,11 +2058,8 @@
       <c r="C79" t="s">
         <v>8</v>
       </c>
-      <c r="E79" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>91</v>
       </c>
@@ -2212,11 +2069,8 @@
       <c r="C80" t="s">
         <v>8</v>
       </c>
-      <c r="E80" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>92</v>
       </c>
@@ -2226,11 +2080,8 @@
       <c r="C81" t="s">
         <v>9</v>
       </c>
-      <c r="E81" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>93</v>
       </c>
@@ -2240,11 +2091,8 @@
       <c r="C82" t="s">
         <v>9</v>
       </c>
-      <c r="E82" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>94</v>
       </c>
@@ -2254,11 +2102,8 @@
       <c r="C83" t="s">
         <v>7</v>
       </c>
-      <c r="E83" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>95</v>
       </c>
@@ -2268,11 +2113,8 @@
       <c r="C84" t="s">
         <v>7</v>
       </c>
-      <c r="E84" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>96</v>
       </c>
@@ -2282,11 +2124,8 @@
       <c r="C85" t="s">
         <v>7</v>
       </c>
-      <c r="E85" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>97</v>
       </c>
@@ -2296,11 +2135,8 @@
       <c r="C86" t="s">
         <v>7</v>
       </c>
-      <c r="E86" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>98</v>
       </c>
@@ -2310,11 +2146,8 @@
       <c r="C87" t="s">
         <v>7</v>
       </c>
-      <c r="E87" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>99</v>
       </c>
@@ -2324,11 +2157,8 @@
       <c r="C88" t="s">
         <v>7</v>
       </c>
-      <c r="E88" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>100</v>
       </c>
@@ -2338,11 +2168,8 @@
       <c r="C89" t="s">
         <v>7</v>
       </c>
-      <c r="E89" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>101</v>
       </c>
@@ -2352,11 +2179,8 @@
       <c r="C90" t="s">
         <v>7</v>
       </c>
-      <c r="E90" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>102</v>
       </c>
@@ -2366,11 +2190,8 @@
       <c r="C91" t="s">
         <v>7</v>
       </c>
-      <c r="E91" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>103</v>
       </c>
@@ -2380,11 +2201,8 @@
       <c r="C92" t="s">
         <v>7</v>
       </c>
-      <c r="E92" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>102</v>
       </c>
@@ -2394,11 +2212,8 @@
       <c r="C93" t="s">
         <v>7</v>
       </c>
-      <c r="E93" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>104</v>
       </c>
@@ -2408,11 +2223,8 @@
       <c r="C94" t="s">
         <v>7</v>
       </c>
-      <c r="E94" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>105</v>
       </c>
@@ -2422,11 +2234,8 @@
       <c r="C95" t="s">
         <v>7</v>
       </c>
-      <c r="E95" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>106</v>
       </c>
@@ -2435,9 +2244,6 @@
       </c>
       <c r="C96" t="s">
         <v>7</v>
-      </c>
-      <c r="E96" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2450,9 +2256,6 @@
       <c r="C97" t="s">
         <v>7</v>
       </c>
-      <c r="E97" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
@@ -2464,9 +2267,6 @@
       <c r="C98" t="s">
         <v>7</v>
       </c>
-      <c r="E98" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
@@ -2478,9 +2278,6 @@
       <c r="C99" t="s">
         <v>7</v>
       </c>
-      <c r="E99" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
@@ -2492,9 +2289,6 @@
       <c r="C100" t="s">
         <v>7</v>
       </c>
-      <c r="E100" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
@@ -2506,9 +2300,6 @@
       <c r="C101" t="s">
         <v>7</v>
       </c>
-      <c r="E101" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
@@ -2520,9 +2311,6 @@
       <c r="C102" t="s">
         <v>7</v>
       </c>
-      <c r="E102" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
@@ -2534,9 +2322,6 @@
       <c r="C103" t="s">
         <v>7</v>
       </c>
-      <c r="E103" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
@@ -2548,9 +2333,6 @@
       <c r="C104" t="s">
         <v>7</v>
       </c>
-      <c r="E104" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
@@ -2562,9 +2344,6 @@
       <c r="C105" t="s">
         <v>7</v>
       </c>
-      <c r="E105" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
@@ -2576,9 +2355,6 @@
       <c r="C106" t="s">
         <v>7</v>
       </c>
-      <c r="E106" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
@@ -2879,9 +2655,6 @@
       <c r="C124" t="s">
         <v>12</v>
       </c>
-      <c r="E124" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
@@ -2893,9 +2666,6 @@
       <c r="C125" t="s">
         <v>12</v>
       </c>
-      <c r="E125" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
@@ -2907,9 +2677,6 @@
       <c r="C126" t="s">
         <v>12</v>
       </c>
-      <c r="E126" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
@@ -2921,9 +2688,6 @@
       <c r="C127" t="s">
         <v>12</v>
       </c>
-      <c r="E127" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
@@ -2935,9 +2699,6 @@
       <c r="C128" t="s">
         <v>12</v>
       </c>
-      <c r="E128" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
@@ -2949,9 +2710,6 @@
       <c r="C129" t="s">
         <v>12</v>
       </c>
-      <c r="E129" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
@@ -2963,9 +2721,6 @@
       <c r="C130" t="s">
         <v>12</v>
       </c>
-      <c r="E130" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
@@ -3232,9 +2987,6 @@
       <c r="C146" t="s">
         <v>7</v>
       </c>
-      <c r="E146" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
@@ -3246,9 +2998,6 @@
       <c r="C147" t="s">
         <v>7</v>
       </c>
-      <c r="E147" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
@@ -3260,9 +3009,6 @@
       <c r="C148" t="s">
         <v>7</v>
       </c>
-      <c r="E148" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
@@ -3274,9 +3020,6 @@
       <c r="C149" t="s">
         <v>7</v>
       </c>
-      <c r="E149" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
@@ -3288,9 +3031,6 @@
       <c r="C150" t="s">
         <v>7</v>
       </c>
-      <c r="E150" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
@@ -3302,9 +3042,6 @@
       <c r="C151" t="s">
         <v>7</v>
       </c>
-      <c r="E151" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
@@ -3316,9 +3053,6 @@
       <c r="C152" t="s">
         <v>7</v>
       </c>
-      <c r="E152" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
@@ -3330,9 +3064,6 @@
       <c r="C153" t="s">
         <v>7</v>
       </c>
-      <c r="E153" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
@@ -3344,9 +3075,6 @@
       <c r="C154" t="s">
         <v>7</v>
       </c>
-      <c r="E154" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
@@ -3358,9 +3086,6 @@
       <c r="C155" t="s">
         <v>7</v>
       </c>
-      <c r="E155" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
@@ -3372,9 +3097,6 @@
       <c r="C156" t="s">
         <v>7</v>
       </c>
-      <c r="E156" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
@@ -3386,9 +3108,6 @@
       <c r="C157" t="s">
         <v>7</v>
       </c>
-      <c r="E157" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
@@ -3400,9 +3119,6 @@
       <c r="C158" t="s">
         <v>7</v>
       </c>
-      <c r="E158" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
@@ -3414,9 +3130,6 @@
       <c r="C159" t="s">
         <v>7</v>
       </c>
-      <c r="E159" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
@@ -3428,11 +3141,8 @@
       <c r="C160" t="s">
         <v>7</v>
       </c>
-      <c r="E160" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>171</v>
       </c>
@@ -3442,11 +3152,8 @@
       <c r="C161" t="s">
         <v>7</v>
       </c>
-      <c r="E161" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>172</v>
       </c>
@@ -3456,11 +3163,8 @@
       <c r="C162" t="s">
         <v>7</v>
       </c>
-      <c r="E162" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>173</v>
       </c>
@@ -3470,11 +3174,8 @@
       <c r="C163" t="s">
         <v>7</v>
       </c>
-      <c r="E163" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>174</v>
       </c>
@@ -3484,11 +3185,8 @@
       <c r="C164" t="s">
         <v>7</v>
       </c>
-      <c r="E164" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>175</v>
       </c>
@@ -3498,11 +3196,8 @@
       <c r="C165" t="s">
         <v>7</v>
       </c>
-      <c r="E165" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>176</v>
       </c>
@@ -3512,11 +3207,8 @@
       <c r="C166" t="s">
         <v>7</v>
       </c>
-      <c r="E166" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>177</v>
       </c>
@@ -3526,11 +3218,8 @@
       <c r="C167" t="s">
         <v>7</v>
       </c>
-      <c r="E167" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>178</v>
       </c>
@@ -3540,11 +3229,8 @@
       <c r="C168" t="s">
         <v>7</v>
       </c>
-      <c r="E168" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>179</v>
       </c>
@@ -3554,11 +3240,8 @@
       <c r="C169" t="s">
         <v>7</v>
       </c>
-      <c r="E169" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>180</v>
       </c>
@@ -3568,11 +3251,8 @@
       <c r="C170" t="s">
         <v>7</v>
       </c>
-      <c r="E170" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>181</v>
       </c>
@@ -3582,11 +3262,8 @@
       <c r="C171" t="s">
         <v>7</v>
       </c>
-      <c r="E171" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>182</v>
       </c>
@@ -3596,11 +3273,8 @@
       <c r="C172" t="s">
         <v>7</v>
       </c>
-      <c r="E172" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>183</v>
       </c>
@@ -3610,11 +3284,8 @@
       <c r="C173" t="s">
         <v>7</v>
       </c>
-      <c r="E173" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>184</v>
       </c>
@@ -3624,11 +3295,8 @@
       <c r="C174" t="s">
         <v>7</v>
       </c>
-      <c r="E174" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>185</v>
       </c>
@@ -3638,11 +3306,8 @@
       <c r="C175" t="s">
         <v>7</v>
       </c>
-      <c r="E175" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>186</v>
       </c>
@@ -3651,9 +3316,6 @@
       </c>
       <c r="C176" t="s">
         <v>7</v>
-      </c>
-      <c r="E176" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -3666,9 +3328,6 @@
       <c r="C177" t="s">
         <v>7</v>
       </c>
-      <c r="E177" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
@@ -3680,9 +3339,6 @@
       <c r="C178" t="s">
         <v>7</v>
       </c>
-      <c r="E178" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
@@ -3710,9 +3366,6 @@
       </c>
       <c r="C180" t="s">
         <v>7</v>
-      </c>
-      <c r="E180" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>